<commit_message>
Updated page creator class to include selects
</commit_message>
<xml_diff>
--- a/Data/ExcelImports/ClientImportJul20.xlsx
+++ b/Data/ExcelImports/ClientImportJul20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/kyle_o'keeffe_ontario_ca/Documents/Documents/02Projects/ProgProj/OACISTestAutomationSelenium/Data/ExcelImports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104845D9184BC25ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8087BAFC-873F-42CF-B891-ABF4F7F7EE8E}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC104845D9184BC25ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D84924F-A0E6-435C-974E-CF90BEC11D19}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,16 +42,16 @@
     <t>21-11-2017</t>
   </si>
   <si>
-    <t>cLNamejultwoF</t>
-  </si>
-  <si>
-    <t>cFNamejultwoF</t>
-  </si>
-  <si>
-    <t>cLNamejultwoG</t>
-  </si>
-  <si>
-    <t>cFNamejultwoG</t>
+    <t>cLNameJulTestA</t>
+  </si>
+  <si>
+    <t>cFNameJulTestA</t>
+  </si>
+  <si>
+    <t>cLNameJulTestB</t>
+  </si>
+  <si>
+    <t>cFNameJultwoB</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>